<commit_message>
added code for linkedlist Module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Register" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="TryEditor" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>scenario</t>
   </si>
@@ -31,7 +32,7 @@
     <t>fieldName</t>
   </si>
   <si>
-    <t>Error message is displayed when the Username field is left empty</t>
+    <t>validate the error message displayed when the username field is left empty</t>
   </si>
   <si>
     <t>pass123</t>
@@ -40,26 +41,53 @@
     <t>Please fill out this field.</t>
   </si>
   <si>
-    <t>Error message is displayed when the Password field is left empty</t>
+    <t>validate the error message displayed when the password field is left empty</t>
   </si>
   <si>
     <t>user1</t>
   </si>
   <si>
-    <t>Error message is displayed when the Password Confirmation field is left empty</t>
+    <t xml:space="preserve"> validate the error message displayed when the confirm password field is left empty</t>
   </si>
   <si>
     <t>user2</t>
   </si>
   <si>
-    <t>Error messages are displayed when all fields are empty during registration.</t>
+    <t xml:space="preserve">validate the error message displayed when all the fields  left empty	</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>Verify that user is able to see output for valid python code</t>
+  </si>
+  <si>
+    <t>print("Hello! Welcome")</t>
+  </si>
+  <si>
+    <t>Hello! Welcome</t>
+  </si>
+  <si>
+    <t>Verify that user receives error for invalid python code</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>NameError: name 'hi' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>Verify that user receives error when click on Run button without entering code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -72,6 +100,7 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -79,6 +108,24 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -115,21 +162,42 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -140,6 +208,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -392,7 +464,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -410,7 +482,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -428,7 +500,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3"/>
@@ -444,4 +516,64 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="35.5"/>
+    <col customWidth="1" min="2" max="2" width="23.5"/>
+    <col customWidth="1" min="3" max="3" width="36.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="6"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made some changes to register file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -47,13 +47,13 @@
     <t>user1</t>
   </si>
   <si>
-    <t xml:space="preserve"> validate the error message displayed when the confirm password field is left empty</t>
+    <t>validate the error message displayed when the confirm password field is left empty</t>
   </si>
   <si>
     <t>user2</t>
   </si>
   <si>
-    <t xml:space="preserve">validate the error message displayed when all the fields  left empty	</t>
+    <t xml:space="preserve">validate the error message displayed when all the fields left empty     </t>
   </si>
   <si>
     <t>Input</t>

</xml_diff>